<commit_message>
Budget Analysis done: check chapter 3
</commit_message>
<xml_diff>
--- a/Documentation/Diagrams/CBA-NPV.xlsx
+++ b/Documentation/Diagrams/CBA-NPV.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10425" windowHeight="4635"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10425" windowHeight="4635" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="CBA" sheetId="2" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
   <si>
     <t>Total:</t>
   </si>
@@ -51,9 +51,6 @@
     <t>Development Cost</t>
   </si>
   <si>
-    <t>One-Time Costs</t>
-  </si>
-  <si>
     <t>Additional donations</t>
   </si>
   <si>
@@ -63,15 +60,9 @@
     <t>COSTS</t>
   </si>
   <si>
-    <t>Tangible</t>
-  </si>
-  <si>
     <t>Total</t>
   </si>
   <si>
-    <t>Intangible</t>
-  </si>
-  <si>
     <t>Faster approval for proposals</t>
   </si>
   <si>
@@ -112,6 +103,18 @@
   </si>
   <si>
     <t>Improve event success rate</t>
+  </si>
+  <si>
+    <t>*Tangible</t>
+  </si>
+  <si>
+    <t>*Intangible</t>
+  </si>
+  <si>
+    <t>*One-Time Cost</t>
+  </si>
+  <si>
+    <t>*Recurring Cost</t>
   </si>
 </sst>
 </file>
@@ -166,7 +169,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -261,16 +264,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="4" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -282,7 +293,6 @@
     <xf numFmtId="165" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -319,6 +329,23 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -635,206 +662,251 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
     <col min="2" max="2" width="9.140625" style="1" customWidth="1"/>
-    <col min="3" max="6" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="11" width="9.140625" style="1"/>
-    <col min="12" max="12" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" style="25" customWidth="1"/>
+    <col min="5" max="6" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="9.140625" style="1"/>
+    <col min="9" max="9" width="10.140625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="9.140625" style="1"/>
+    <col min="11" max="11" width="10.42578125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="10.140625" style="25" bestFit="1" customWidth="1"/>
     <col min="13" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A1" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="H1" s="16" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
-      <c r="K1" s="16"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A3" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="16"/>
-      <c r="C3" s="16"/>
-      <c r="H3" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="I3" s="16"/>
-      <c r="J3" s="16"/>
-      <c r="K3" s="16"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A5" s="15" t="s">
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="E1" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="25"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E2" s="28"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
+      <c r="I2" s="25"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="14"/>
+      <c r="C3" s="14"/>
+      <c r="E3" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" s="30"/>
+      <c r="G3" s="30"/>
+      <c r="H3" s="30"/>
+      <c r="I3" s="25"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E4" s="28"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="27"/>
+      <c r="I4" s="25"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="15"/>
-      <c r="C5" s="15"/>
-      <c r="D5" s="1">
+      <c r="B5" s="13"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="25">
         <v>50000</v>
       </c>
-      <c r="H5" s="15" t="s">
+      <c r="E5" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="I5" s="15"/>
-      <c r="J5" s="15"/>
-      <c r="K5" s="15"/>
-      <c r="L5" s="1">
+      <c r="F5" s="32"/>
+      <c r="G5" s="32"/>
+      <c r="H5" s="32"/>
+      <c r="I5" s="25">
         <f>215*2*12</f>
         <v>5160</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A6" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="B6" s="15"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="1">
-        <v>3275</v>
-      </c>
-      <c r="H6" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="I6" s="15"/>
-      <c r="J6" s="15"/>
-      <c r="K6" s="15"/>
-      <c r="L6" s="1">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C6" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D6" s="26">
+        <f>D5</f>
+        <v>50000</v>
+      </c>
+      <c r="E6" s="31" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" s="32"/>
+      <c r="G6" s="32"/>
+      <c r="H6" s="32"/>
+      <c r="I6" s="25">
         <f>(1300/60)*2000</f>
         <v>43333.333333333336</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="C7" s="3" t="s">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E7" s="28"/>
+      <c r="F7" s="27"/>
+      <c r="G7" s="27"/>
+      <c r="H7" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="D7" s="3">
-        <f>SUM(D5:D6)</f>
-        <v>53275</v>
-      </c>
-      <c r="K7" s="3" t="s">
+      <c r="I7" s="26">
+        <f>SUM(I5:I6)</f>
+        <v>48493.333333333336</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E8" s="28"/>
+      <c r="F8" s="27"/>
+      <c r="G8" s="27"/>
+      <c r="H8" s="27"/>
+      <c r="I8" s="25"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="14"/>
+      <c r="C9" s="14"/>
+      <c r="E9" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="F9" s="30"/>
+      <c r="G9" s="30"/>
+      <c r="H9" s="30"/>
+      <c r="I9" s="25"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E10" s="28"/>
+      <c r="F10" s="27"/>
+      <c r="G10" s="27"/>
+      <c r="H10" s="27"/>
+      <c r="I10" s="25"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" s="13"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="25">
+        <v>1148</v>
+      </c>
+      <c r="E11" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" s="32"/>
+      <c r="G11" s="32"/>
+      <c r="H11" s="32"/>
+      <c r="I11" s="25">
         <v>0</v>
       </c>
-      <c r="L7" s="4">
-        <f>SUM(L5:L6)</f>
-        <v>48493.333333333336</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="H9" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="I9" s="16"/>
-      <c r="J9" s="16"/>
-      <c r="K9" s="16"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A10" s="14"/>
-      <c r="B10" s="14"/>
-      <c r="C10" s="14"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="H11" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="I11" s="15"/>
-      <c r="J11" s="15"/>
-      <c r="K11" s="15"/>
-      <c r="L11" s="1">
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C12" s="3" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A12" s="13"/>
-      <c r="B12" s="13"/>
-      <c r="C12" s="13"/>
-      <c r="H12" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="I12" s="15"/>
-      <c r="J12" s="15"/>
-      <c r="K12" s="15"/>
-      <c r="L12" s="1">
+      <c r="D12" s="26">
+        <f>D11</f>
+        <v>1148</v>
+      </c>
+      <c r="E12" s="31" t="s">
+        <v>11</v>
+      </c>
+      <c r="F12" s="32"/>
+      <c r="G12" s="32"/>
+      <c r="H12" s="32"/>
+      <c r="I12" s="25">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="H13" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="I13" s="15"/>
-      <c r="J13" s="15"/>
-      <c r="K13" s="15"/>
-      <c r="L13" s="1">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E13" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="F13" s="32"/>
+      <c r="G13" s="32"/>
+      <c r="H13" s="32"/>
+      <c r="I13" s="25">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A14" s="13"/>
-      <c r="B14" s="13"/>
-      <c r="C14" s="13"/>
-      <c r="H14" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="I14" s="15"/>
-      <c r="J14" s="15"/>
-      <c r="K14" s="15"/>
-      <c r="L14" s="1">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" s="12"/>
+      <c r="B14" s="12"/>
+      <c r="C14" s="12"/>
+      <c r="E14" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="F14" s="32"/>
+      <c r="G14" s="32"/>
+      <c r="H14" s="32"/>
+      <c r="I14" s="25">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A15" s="13"/>
-      <c r="B15" s="13"/>
-      <c r="C15" s="13"/>
-      <c r="H15" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="I15" s="15"/>
-      <c r="J15" s="15"/>
-      <c r="K15" s="15"/>
-      <c r="L15" s="1">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15" s="12"/>
+      <c r="B15" s="12"/>
+      <c r="C15" s="12"/>
+      <c r="E15" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="F15" s="32"/>
+      <c r="G15" s="32"/>
+      <c r="H15" s="32"/>
+      <c r="I15" s="25">
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="K16" s="3" t="s">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E16" s="28"/>
+      <c r="F16" s="27"/>
+      <c r="G16" s="27"/>
+      <c r="H16" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="L16" s="3">
-        <f>SUM(L11:L15)</f>
+      <c r="I16" s="26">
+        <f>SUM(I11:I15)</f>
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="14">
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="H15:K15"/>
-    <mergeCell ref="H3:K3"/>
-    <mergeCell ref="H1:K1"/>
+  <mergeCells count="15">
+    <mergeCell ref="E15:H15"/>
+    <mergeCell ref="E3:H3"/>
+    <mergeCell ref="E1:H1"/>
     <mergeCell ref="A1:C1"/>
-    <mergeCell ref="H9:K9"/>
-    <mergeCell ref="H14:K14"/>
-    <mergeCell ref="H13:K13"/>
-    <mergeCell ref="H12:K12"/>
-    <mergeCell ref="H11:K11"/>
-    <mergeCell ref="H6:K6"/>
-    <mergeCell ref="H5:K5"/>
+    <mergeCell ref="E9:H9"/>
+    <mergeCell ref="E14:H14"/>
+    <mergeCell ref="E13:H13"/>
+    <mergeCell ref="E12:H12"/>
+    <mergeCell ref="E11:H11"/>
+    <mergeCell ref="E6:H6"/>
+    <mergeCell ref="E5:H5"/>
     <mergeCell ref="A5:C5"/>
     <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="A11:C11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -845,8 +917,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10:F10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -858,294 +930,294 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="4">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="5"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="23"/>
+      <c r="B4" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="22"/>
+      <c r="D4" s="22"/>
+      <c r="E4" s="22"/>
+      <c r="F4" s="22"/>
+      <c r="G4" s="24" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="23"/>
+      <c r="B5" s="6">
+        <v>0</v>
+      </c>
+      <c r="C5" s="6">
+        <v>1</v>
+      </c>
+      <c r="D5" s="6">
+        <v>2</v>
+      </c>
+      <c r="E5" s="6">
+        <v>3</v>
+      </c>
+      <c r="F5" s="6">
+        <v>4</v>
+      </c>
+      <c r="G5" s="24"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="8">
+        <f>CBA!D6+CBA!D12</f>
+        <v>51148</v>
+      </c>
+      <c r="C6" s="8">
+        <f>CBA!D12</f>
+        <v>1148</v>
+      </c>
+      <c r="D6" s="8">
+        <f>CBA!D12</f>
+        <v>1148</v>
+      </c>
+      <c r="E6" s="8">
+        <f>CBA!D12</f>
+        <v>1148</v>
+      </c>
+      <c r="F6" s="8">
+        <f>CBA!D12</f>
+        <v>1148</v>
+      </c>
+      <c r="G6" s="21"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="9">
+        <f>1/(1+0.1)^B5</f>
+        <v>1</v>
+      </c>
+      <c r="C7" s="9">
+        <f t="shared" ref="C7:F7" si="0">1/(1+0.1)^C5</f>
+        <v>0.90909090909090906</v>
+      </c>
+      <c r="D7" s="9">
+        <f t="shared" si="0"/>
+        <v>0.82644628099173545</v>
+      </c>
+      <c r="E7" s="9">
+        <f t="shared" si="0"/>
+        <v>0.75131480090157754</v>
+      </c>
+      <c r="F7" s="9">
+        <f t="shared" si="0"/>
+        <v>0.68301345536507052</v>
+      </c>
+      <c r="G7" s="20"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="5">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="17" t="s">
+      <c r="B8" s="8">
+        <f>B6*B7</f>
+        <v>51148</v>
+      </c>
+      <c r="C8" s="8">
+        <f>C6*C7</f>
+        <v>1043.6363636363635</v>
+      </c>
+      <c r="D8" s="8">
+        <f>D6*D7</f>
+        <v>948.76033057851225</v>
+      </c>
+      <c r="E8" s="8">
+        <f>E6*E7</f>
+        <v>862.50939143501103</v>
+      </c>
+      <c r="F8" s="8">
+        <f>F6*F7</f>
+        <v>784.09944675910094</v>
+      </c>
+      <c r="G8" s="10">
+        <f>SUM(B8:F8)</f>
+        <v>54787.005532408984</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="16"/>
+      <c r="B9" s="17"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="18"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="8">
+        <v>0</v>
+      </c>
+      <c r="C10" s="8">
+        <f>CBA!I7</f>
+        <v>48493.333333333336</v>
+      </c>
+      <c r="D10" s="8">
+        <f>CBA!I7</f>
+        <v>48493.333333333336</v>
+      </c>
+      <c r="E10" s="8">
+        <f>CBA!I7</f>
+        <v>48493.333333333336</v>
+      </c>
+      <c r="F10" s="8">
+        <f>CBA!I7</f>
+        <v>48493.333333333336</v>
+      </c>
+      <c r="G10" s="19"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="6"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="25"/>
-      <c r="B4" s="24" t="s">
+      <c r="B11" s="9">
+        <f>1/(1+0.1)^B5</f>
+        <v>1</v>
+      </c>
+      <c r="C11" s="9">
+        <f t="shared" ref="C11:F11" si="1">1/(1+0.1)^C5</f>
+        <v>0.90909090909090906</v>
+      </c>
+      <c r="D11" s="9">
+        <f t="shared" si="1"/>
+        <v>0.82644628099173545</v>
+      </c>
+      <c r="E11" s="9">
+        <f t="shared" si="1"/>
+        <v>0.75131480090157754</v>
+      </c>
+      <c r="F11" s="9">
+        <f t="shared" si="1"/>
+        <v>0.68301345536507052</v>
+      </c>
+      <c r="G11" s="20"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="26" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="25"/>
-      <c r="B5" s="7">
-        <v>0</v>
-      </c>
-      <c r="C5" s="7">
-        <v>1</v>
-      </c>
-      <c r="D5" s="7">
-        <v>2</v>
-      </c>
-      <c r="E5" s="7">
-        <v>3</v>
-      </c>
-      <c r="F5" s="7">
-        <v>4</v>
-      </c>
-      <c r="G5" s="26"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="9">
-        <f>CBA!D7</f>
-        <v>53275</v>
-      </c>
-      <c r="C6" s="9">
-        <f>CBA!D13</f>
-        <v>0</v>
-      </c>
-      <c r="D6" s="9">
-        <f>CBA!D13</f>
-        <v>0</v>
-      </c>
-      <c r="E6" s="9">
-        <f>CBA!D13</f>
-        <v>0</v>
-      </c>
-      <c r="F6" s="9">
-        <f>CBA!D13</f>
-        <v>0</v>
-      </c>
-      <c r="G6" s="23"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" s="10">
-        <f>1/(1+0.08)^B5</f>
-        <v>1</v>
-      </c>
-      <c r="C7" s="10">
-        <f>1/(1+0.08)^C5</f>
-        <v>0.92592592592592582</v>
-      </c>
-      <c r="D7" s="10">
-        <f>1/(1+0.08)^D5</f>
-        <v>0.85733882030178321</v>
-      </c>
-      <c r="E7" s="10">
-        <f>1/(1+0.08)^E5</f>
-        <v>0.79383224102016958</v>
-      </c>
-      <c r="F7" s="10">
-        <f>1/(1+0.08)^F5</f>
-        <v>0.73502985279645328</v>
-      </c>
-      <c r="G7" s="22"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" s="9">
-        <f>B6*B7</f>
-        <v>53275</v>
-      </c>
-      <c r="C8" s="9">
-        <f>C6*C7</f>
-        <v>0</v>
-      </c>
-      <c r="D8" s="9">
-        <f>D6*D7</f>
-        <v>0</v>
-      </c>
-      <c r="E8" s="9">
-        <f>E6*E7</f>
-        <v>0</v>
-      </c>
-      <c r="F8" s="9">
-        <f>F6*F7</f>
-        <v>0</v>
-      </c>
-      <c r="G8" s="11">
-        <f>SUM(B8:F8)</f>
-        <v>53275</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="18"/>
-      <c r="B9" s="19"/>
-      <c r="C9" s="19"/>
-      <c r="D9" s="19"/>
-      <c r="E9" s="19"/>
-      <c r="F9" s="19"/>
-      <c r="G9" s="20"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="B10" s="9">
-        <v>0</v>
-      </c>
-      <c r="C10" s="9">
-        <f>CBA!L7</f>
-        <v>48493.333333333336</v>
-      </c>
-      <c r="D10" s="9">
-        <f>CBA!L7</f>
-        <v>48493.333333333336</v>
-      </c>
-      <c r="E10" s="9">
-        <f>CBA!L7</f>
-        <v>48493.333333333336</v>
-      </c>
-      <c r="F10" s="9">
-        <f>CBA!L7</f>
-        <v>48493.333333333336</v>
-      </c>
-      <c r="G10" s="21"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="B11" s="10">
-        <f>1/(1+0.08)^B5</f>
-        <v>1</v>
-      </c>
-      <c r="C11" s="10">
-        <f>1/(1+0.08)^C5</f>
-        <v>0.92592592592592582</v>
-      </c>
-      <c r="D11" s="10">
-        <f>1/(1+0.08)^D5</f>
-        <v>0.85733882030178321</v>
-      </c>
-      <c r="E11" s="10">
-        <f>1/(1+0.08)^E5</f>
-        <v>0.79383224102016958</v>
-      </c>
-      <c r="F11" s="10">
-        <f>1/(1+0.08)^F5</f>
-        <v>0.73502985279645328</v>
-      </c>
-      <c r="G11" s="22"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="B12" s="9">
+      <c r="B12" s="8">
         <f>B10*B11</f>
         <v>0</v>
       </c>
-      <c r="C12" s="9">
-        <f t="shared" ref="C12:F12" si="0">C10*C11</f>
-        <v>44901.234567901229</v>
-      </c>
-      <c r="D12" s="9">
-        <f t="shared" si="0"/>
-        <v>41575.217192501143</v>
-      </c>
-      <c r="E12" s="9">
-        <f t="shared" si="0"/>
-        <v>38495.57147453809</v>
-      </c>
-      <c r="F12" s="9">
-        <f t="shared" si="0"/>
-        <v>35644.047661609344</v>
-      </c>
-      <c r="G12" s="11">
+      <c r="C12" s="8">
+        <f t="shared" ref="C12:F12" si="2">C10*C11</f>
+        <v>44084.848484848488</v>
+      </c>
+      <c r="D12" s="8">
+        <f t="shared" si="2"/>
+        <v>40077.134986225894</v>
+      </c>
+      <c r="E12" s="8">
+        <f t="shared" si="2"/>
+        <v>36433.759078387171</v>
+      </c>
+      <c r="F12" s="8">
+        <f t="shared" si="2"/>
+        <v>33121.599162170154</v>
+      </c>
+      <c r="G12" s="10">
         <f>SUM(B12:F12)</f>
-        <v>160616.07089654979</v>
+        <v>153717.34171163169</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="18"/>
-      <c r="B13" s="19"/>
-      <c r="C13" s="19"/>
-      <c r="D13" s="19"/>
-      <c r="E13" s="19"/>
-      <c r="F13" s="19"/>
-      <c r="G13" s="20"/>
+      <c r="A13" s="16"/>
+      <c r="B13" s="17"/>
+      <c r="C13" s="17"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="17"/>
+      <c r="G13" s="18"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="B14" s="9">
+      <c r="A14" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="8">
         <f>B12-B8</f>
-        <v>-53275</v>
-      </c>
-      <c r="C14" s="9">
-        <f t="shared" ref="C14:F14" si="1">C12-C8</f>
-        <v>44901.234567901229</v>
-      </c>
-      <c r="D14" s="9">
-        <f t="shared" si="1"/>
-        <v>41575.217192501143</v>
-      </c>
-      <c r="E14" s="9">
-        <f t="shared" si="1"/>
-        <v>38495.57147453809</v>
-      </c>
-      <c r="F14" s="9">
-        <f t="shared" si="1"/>
-        <v>35644.047661609344</v>
-      </c>
-      <c r="G14" s="21"/>
+        <v>-51148</v>
+      </c>
+      <c r="C14" s="8">
+        <f t="shared" ref="C14:F14" si="3">C12-C8</f>
+        <v>43041.212121212127</v>
+      </c>
+      <c r="D14" s="8">
+        <f t="shared" si="3"/>
+        <v>39128.374655647385</v>
+      </c>
+      <c r="E14" s="8">
+        <f t="shared" si="3"/>
+        <v>35571.249686952156</v>
+      </c>
+      <c r="F14" s="8">
+        <f t="shared" si="3"/>
+        <v>32337.499715411053</v>
+      </c>
+      <c r="G14" s="19"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B15" s="9">
+      <c r="A15" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" s="8">
         <f>B14</f>
-        <v>-53275</v>
-      </c>
-      <c r="C15" s="9">
+        <v>-51148</v>
+      </c>
+      <c r="C15" s="8">
         <f>B15+C14</f>
-        <v>-8373.7654320987713</v>
-      </c>
-      <c r="D15" s="9">
+        <v>-8106.7878787878726</v>
+      </c>
+      <c r="D15" s="8">
         <f>C15+D14</f>
-        <v>33201.451760402371</v>
-      </c>
-      <c r="E15" s="9">
+        <v>31021.586776859513</v>
+      </c>
+      <c r="E15" s="8">
         <f>D15+E14</f>
-        <v>71697.023234940454</v>
-      </c>
-      <c r="F15" s="9">
+        <v>66592.836463811662</v>
+      </c>
+      <c r="F15" s="8">
         <f>E15+F14</f>
-        <v>107341.07089654979</v>
-      </c>
-      <c r="G15" s="22"/>
+        <v>98930.336179222708</v>
+      </c>
+      <c r="G15" s="20"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="3"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B17" s="12">
+        <v>18</v>
+      </c>
+      <c r="B17" s="11">
         <f>((G12-G8)/G8)</f>
-        <v>2.0148488202074106</v>
+        <v>1.8057262888861658</v>
       </c>
     </row>
   </sheetData>

</xml_diff>